<commit_message>
Fixed garbage at bottom of chem.dat. Control file has slashes in PC mode (\). Seawater.xlsx has comparison of n-averaged observations, need flow-weighted averages.
git-svn-id: svn://136.177.114.72/svn_GW/webmod/trunk@9980 1feff8c3-07ed-0310-ac33-dd36852eb9cd
</commit_message>
<xml_diff>
--- a/projects/icacos/References/Seawater.xlsx
+++ b/projects/icacos/References/Seawater.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="88">
   <si>
     <r>
       <rPr>
@@ -860,13 +860,40 @@
     <t>pH</t>
   </si>
   <si>
-    <t>S(6)</t>
-  </si>
-  <si>
     <t>Alkalinity</t>
   </si>
   <si>
     <t>Mol ratio</t>
+  </si>
+  <si>
+    <t>Georges precip 9/21-22/1998</t>
+  </si>
+  <si>
+    <t>Milliero 2008</t>
+  </si>
+  <si>
+    <t>QCDave &amp; PHREEQC</t>
+  </si>
+  <si>
+    <t>SO4</t>
+  </si>
+  <si>
+    <t>NO3</t>
+  </si>
+  <si>
+    <t>Average concentrations (n samples - mg/L)</t>
+  </si>
+  <si>
+    <t>mg/L normalized to 455uM Cl</t>
+  </si>
+  <si>
+    <t>Stream</t>
+  </si>
+  <si>
+    <t>Precip</t>
+  </si>
+  <si>
+    <t>Flow weighted conc (mg/L)?</t>
   </si>
 </sst>
 </file>
@@ -878,7 +905,7 @@
     <numFmt numFmtId="165" formatCode="###0.00000000;###0.00000000"/>
     <numFmt numFmtId="166" formatCode="###0.0;###0.0"/>
     <numFmt numFmtId="167" formatCode="###0;###0"/>
-    <numFmt numFmtId="172" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -965,7 +992,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1022,11 +1049,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1333,20 +1381,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
     <col min="7" max="7" width="23.33203125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
@@ -1383,7 +1429,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I4" s="15" t="s">
         <v>33</v>
@@ -1813,7 +1859,7 @@
         <v>1.0820328160693062E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
@@ -1848,7 +1894,7 @@
         <v>1.1302317839467473E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
@@ -1883,7 +1929,7 @@
         <v>1.61970765098822E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>29</v>
       </c>
@@ -1918,7 +1964,7 @@
         <v>3.5531510513096132E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>30</v>
       </c>
@@ -1943,156 +1989,358 @@
         <v>2.0513498405044728</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B25" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B26" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="D26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="E26" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="F26" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="G26" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="H26" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="I26" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="H26" s="18" t="s">
+      <c r="J26" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="I26" s="18" t="s">
+      <c r="K26" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="J26" s="18" t="s">
+      <c r="L26" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27">
+        <v>7.49</v>
+      </c>
+      <c r="C27">
         <f>J7</f>
         <v>0.34348531491389384</v>
       </c>
-      <c r="B27">
+      <c r="D27">
         <f>J6</f>
         <v>1.0700202730678954</v>
       </c>
-      <c r="C27">
+      <c r="E27">
         <f>J5</f>
         <v>8.9866914101469693</v>
       </c>
-      <c r="D27">
+      <c r="F27">
         <f>J8</f>
         <v>0.33266537691495818</v>
       </c>
-      <c r="F27">
+      <c r="H27">
         <f>SUM(J12:J14)</f>
         <v>0.15539988926774173</v>
       </c>
-      <c r="G27">
+      <c r="I27">
         <f>J10</f>
         <v>16.131115000000001</v>
       </c>
-      <c r="H27">
+      <c r="J27">
         <f>J11</f>
         <v>2.2608334582726823</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="20">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="21">
+        <v>7.4920017100000003</v>
+      </c>
+      <c r="C28" s="22">
+        <f>C31</f>
+        <v>0.3431140781</v>
+      </c>
+      <c r="D28" s="22">
+        <f>C34</f>
+        <v>1.075029751</v>
+      </c>
+      <c r="E28" s="22">
+        <f>C35</f>
+        <v>8.961077843</v>
+      </c>
+      <c r="F28" s="22">
+        <f>C33</f>
+        <v>0.33212910159999998</v>
+      </c>
+      <c r="H28" s="22">
+        <f>C30</f>
         <v>9.6763793799999998E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="I28" s="22">
+        <f>C32</f>
+        <v>16.12815325</v>
+      </c>
+      <c r="J28" s="22">
+        <f>C36</f>
+        <v>2.2569133670000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C29" s="23">
+        <f>ROUND(C28,2)</f>
+        <v>0.34</v>
+      </c>
+      <c r="D29" s="23">
+        <f t="shared" ref="D29:K29" si="5">ROUND(D28,2)</f>
+        <v>1.08</v>
+      </c>
+      <c r="E29" s="23">
+        <f t="shared" si="5"/>
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="F29" s="23">
+        <f t="shared" si="5"/>
+        <v>0.33</v>
+      </c>
+      <c r="G29" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="23">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="I29" s="23">
+        <f t="shared" si="5"/>
+        <v>16.13</v>
+      </c>
+      <c r="J29" s="23">
+        <f t="shared" si="5"/>
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="K29" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="20">
+        <v>9.6763793799999998E-2</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" s="28"/>
+    </row>
+    <row r="31" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="20">
+      <c r="C31" s="20">
         <v>0.3431140781</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="E31" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="G31" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+    </row>
+    <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="20">
+      <c r="C32" s="20">
         <v>16.12815325</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="D32" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32">
+        <v>7.49</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="20">
+      <c r="C33" s="20">
         <v>0.33212910159999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="D33" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33">
+        <v>0.34</v>
+      </c>
+      <c r="F33">
+        <v>2.6457142857142864</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="20">
+      <c r="C34" s="20">
         <v>1.075029751</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="D34" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34">
+        <v>1.08</v>
+      </c>
+      <c r="F34">
+        <v>1.4557142857142857</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="20">
-        <v>1.016564617</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B36" s="20">
+      <c r="C35" s="20">
+        <v>8.961077843</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="F35">
+        <v>11.254285714285714</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B36" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="20">
         <v>2.2569133670000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="D36" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36">
+        <v>0.33</v>
+      </c>
+      <c r="F36">
+        <v>1.8325000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="20">
+      <c r="C37" s="20">
         <v>3.561795428E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="D37" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="21">
+      <c r="C38" s="21">
         <v>7.4920017100000003</v>
       </c>
+      <c r="D38" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38">
+        <v>0.1</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D39" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39">
+        <v>16.13</v>
+      </c>
+      <c r="F39">
+        <v>33.906666666666659</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D40" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E40">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="F40">
+        <v>3.4285714285714279</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D41" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>1.8000000000000002E-2</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F30:G30"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>